<commit_message>
add push ios automation
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="596" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="596" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="conf5" sheetId="2" r:id="rId2"/>
-    <sheet name="bind" sheetId="3" r:id="rId3"/>
-    <sheet name="push" sheetId="4" r:id="rId4"/>
+    <sheet name="bindAndroid" sheetId="3" r:id="rId3"/>
+    <sheet name="pushAndroid" sheetId="4" r:id="rId4"/>
+    <sheet name="bindIOS" sheetId="5" r:id="rId5"/>
+    <sheet name="pushIOS" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="205">
   <si>
     <t>ApiUrl</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -416,43 +418,95 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>status_Exp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4320</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求缺少必要参数:appkey,不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error_Exp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求缺少必要参数:apppkg,不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求缺少必要参数:plat,不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求缺少必要参数:platVersion,不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求缺少必要参数:duid,不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>status_Exp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4320</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请求缺少必要参数:appkey,不能为空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>error_Exp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请求缺少必要参数:apppkg,不能为空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请求缺少必要参数:plat,不能为空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请求缺少必要参数:platVersion,不能为空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>请求缺少必要参数:duid,不能为空</t>
+    <t>请求缺少必要参数:product,不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/auth/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/v3/bind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/v3/push/createPush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>domainList,registrationId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pushTarget_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pushNotify_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"notifyId":"1065a3de-597a-4e2b-a83c-02e882c68438"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2dbe655e88c80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2dbe655e88c80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DependID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -460,59 +514,197 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>请求缺少必要参数:product,不能为空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/auth/login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/v3/bind</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/v3/push/createPush</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>domainList,registrationId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pushTarget_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pushNotify_Req</t>
+    <t>header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isLocal_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pushOperator_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isLocal,appkey,pushTarget,pushNotify,pushOperator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key=2dbe655e88c80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tcpFlag_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>channel_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vivo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vivo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>openPush_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.mob.mobpush.demo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>registrationId_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceTokenNew_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regId_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceToken_Req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3bb46a72a653c0781b4360ff40355c02b500fd9d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15858120640241856854784</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65ou9maz9e7m4n4</t>
+  </si>
+  <si>
+    <t>65ou9maz9e7m4n4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65ou9maz9e7m4n4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"rids":["65ou9maz9e7m4n4"],"tagsType":1,"target":4}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android-通知推送-RID方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android-通知推送-广播方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"target":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"Android-通知-RID-自动化","extras":{},"extrasMapList":[],"iosProduction":1,"offlineSeconds":0,"plats":[1],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"Android-通知-广播-自动化","extras":{},"extrasMapList":[],"offlineSeconds":0,"plats":[1],"taskCron":0,"title":"V3新接口测试","type":1}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{"notifyId":"1065a3de-597a-4e2b-a83c-02e882c68438"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2dbe655e88c80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"content":"推送V3接口自动化","extras":{},"extrasMapList":[],"iosProduction":1,"offlineSeconds":0,"plats":[1],"taskCron":0,"title":"V3新接口测试","type":1}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2dbe655e88c80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DependID</t>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"target":3,"tags":["自动化标签1","自动化标签2"],"tagsType":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"Android-通知-标签交集-自动化","extras":{},"extrasMapList":[],"offlineSeconds":0,"plats":[1],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android-通知推送-自定义标签-并集方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android-通知推送-自定义标签-交集方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"target":3,"tags":["自动化标签1","自动化标签2"],"tagsType":2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"Android-通知-标签并集-自动化","extras":{},"extrasMapList":[],"offlineSeconds":0,"plats":[1],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android-通知推送-自定义别名方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"target":2,"alias":["自动化别名1","自动化别名2"]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"Android-通知-别名-自动化","extras":{},"extrasMapList":[],"offlineSeconds":0,"plats":[1],"taskCron":0,"title":"V3新接口测试","type":1}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -520,67 +712,50 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bind</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>header</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>header</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>header</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isLocal_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pushOperator_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isLocal,appkey,pushTarget,pushNotify,pushOperator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key=2dbe655e88c80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tcpFlag_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>channel_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vivo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vivo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>openPush_Req</t>
+    <t>iOS-通知推送-RID方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iOS-通知推送-广播方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iOS-通知推送-自定义标签-交集方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iOS-通知推送-自定义标签-并集方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iOS-通知推送-自定义别名方式，所有字段均不为空，返回接口结果与预期一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bindAndroid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key=moba6b6c6d6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moba6b6c6d6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moba6b6c6d6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -588,50 +763,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>com.mob.mobpush.demo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>registrationId_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>deviceTokenNew_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>regId_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>deviceToken_Req</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.0.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3bb46a72a653c0781b4360ff40355c02b500fd9d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>15858120640241856854784</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65ou9maz9e7m4n4</t>
-  </si>
-  <si>
-    <t>65ou9maz9e7m4n4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>65ou9maz9e7m4n4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"rids":["65ou9maz9e7m4n4"],"tagsType":1,"target":4}</t>
+    <t>com.mob.MobPush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13.5.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>80f973fda27df60974e9237a8143d98b7b7d3d30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12D326C3629030A73031E19AB732D08945623C1483B9E18388D82045337E9313</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0d43b51e718908096734377b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apns</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"rids":["0d43b51e718908096734377b"],"tagsType":1,"target":4}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"iOS-通知-别名-自动化","extras":{},"extrasMapList":[],"iosProduction":1,"offlineSeconds":0,"plats":[2],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"iOS-通知-标签并集-自动化","extras":{},"extrasMapList":[],"iosProduction":1,"offlineSeconds":0,"plats":[2],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"iOS-通知-标签交集-自动化","extras":{},"extrasMapList":[],"iosProduction":1,"offlineSeconds":0,"plats":[2],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"iOS-通知-广播-自动化","extras":{},"extrasMapList":[],"iosProduction":1,"offlineSeconds":0,"plats":[2],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content":"iOS-通知-RID-自动化","extras":{},"extrasMapList":[],"iosProduction":1,"offlineSeconds":0,"plats":[2],"taskCron":0,"title":"V3新接口测试","type":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bindIOS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0d43b51e718908096734377b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"target":3,"tags":["test"],"tagsType":2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"target":3,"tags":["test"],"tagsType":1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"target":2,"alias":["test"]}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -760,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -846,6 +1046,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1129,7 +1332,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1149,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -1176,7 +1379,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="16"/>
     </row>
@@ -1197,7 +1400,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>34</v>
@@ -1389,7 +1592,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1444,7 +1647,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="16"/>
     </row>
@@ -1465,7 +1668,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>42</v>
@@ -1849,13 +2052,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.625" style="3"/>
+    <col min="1" max="1" width="19.625" style="3" customWidth="1"/>
     <col min="2" max="2" width="71.375" style="3" customWidth="1"/>
     <col min="3" max="3" width="6.25" style="27" customWidth="1"/>
     <col min="4" max="4" width="19.625" style="27"/>
@@ -1881,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.15">
@@ -1908,7 +2111,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="16"/>
     </row>
@@ -1929,7 +2132,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>42</v>
@@ -1956,31 +2159,31 @@
         <v>97</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="S7" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="T7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U7" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1994,55 +2197,55 @@
         <v>7</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H8" s="21" t="s">
         <v>94</v>
       </c>
       <c r="I8" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q8" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="J8" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="K8" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="M8" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="N8" s="21" t="s">
+      <c r="R8" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O8" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P8" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R8" s="21" t="s">
+      <c r="S8" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S8" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T8" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U8" s="24"/>
     </row>
@@ -2057,56 +2260,56 @@
         <v>7</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>94</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L9" s="21" t="s">
         <v>94</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="R9" s="21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="T9" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="U9" s="24" t="s">
         <v>103</v>
-      </c>
-      <c r="U9" s="24" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2120,53 +2323,53 @@
         <v>7</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>94</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N10" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R10" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P10" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q10" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R10" s="21" t="s">
+      <c r="S10" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S10" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T10" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U10" s="24"/>
     </row>
@@ -2181,56 +2384,56 @@
         <v>7</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21" t="s">
-        <v>94</v>
+        <v>174</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K11" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L11" s="21" t="s">
         <v>94</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N11" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R11" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O11" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P11" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q11" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R11" s="21" t="s">
+      <c r="S11" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S11" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T11" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U11" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2244,56 +2447,56 @@
         <v>7</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L12" s="21" t="s">
         <v>94</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N12" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R12" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O12" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P12" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q12" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R12" s="21" t="s">
+      <c r="S12" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S12" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T12" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U12" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2307,56 +2510,56 @@
         <v>84</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L13" s="21" t="s">
         <v>94</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N13" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R13" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P13" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q13" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R13" s="21" t="s">
+      <c r="S13" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S13" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T13" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U13" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2370,53 +2573,53 @@
         <v>7</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J14" s="21"/>
       <c r="K14" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P14" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="L14" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="M14" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="N14" s="21" t="s">
+      <c r="Q14" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R14" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O14" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P14" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q14" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R14" s="21" t="s">
+      <c r="S14" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S14" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T14" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U14" s="24"/>
     </row>
@@ -2431,61 +2634,61 @@
         <v>7</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K15" s="21"/>
       <c r="L15" s="21" t="s">
         <v>94</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N15" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R15" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O15" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P15" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q15" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R15" s="21" t="s">
+      <c r="S15" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S15" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T15" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U15" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>91</v>
@@ -2494,56 +2697,56 @@
         <v>7</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L16" s="21"/>
       <c r="M16" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N16" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R16" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="O16" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="P16" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q16" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="R16" s="21" t="s">
+      <c r="S16" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="S16" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="T16" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U16" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2555,17 +2758,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13" style="3" customWidth="1"/>
-    <col min="2" max="2" width="69.25" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9" style="27"/>
+    <col min="2" max="2" width="76.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9" style="27" customWidth="1"/>
     <col min="4" max="4" width="17.875" style="27" customWidth="1"/>
     <col min="5" max="5" width="13" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.875" style="3" customWidth="1"/>
@@ -2573,7 +2776,8 @@
     <col min="8" max="8" width="16.75" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="3"/>
+    <col min="11" max="11" width="9" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
@@ -2581,7 +2785,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
@@ -2597,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -2605,15 +2809,15 @@
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>126</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
@@ -2621,7 +2825,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2635,22 +2839,22 @@
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>52</v>
@@ -2661,29 +2865,149 @@
         <v>58</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="F8" s="31" t="s">
-        <v>121</v>
-      </c>
       <c r="G8" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="I8" s="21" t="s">
+      <c r="D9" s="33"/>
+      <c r="E9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="21" t="s">
-        <v>102</v>
+      <c r="F12" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2691,4 +3015,911 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S16"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="71.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.25" style="27" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="27"/>
+    <col min="5" max="5" width="15.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21.125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.25" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.625" style="3"/>
+    <col min="10" max="10" width="12.375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.625" style="3"/>
+    <col min="12" max="12" width="15.625" style="3" customWidth="1"/>
+    <col min="13" max="15" width="19.625" style="3"/>
+    <col min="16" max="16" width="13.5" style="3" customWidth="1"/>
+    <col min="17" max="17" width="15.625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="19.625" style="3"/>
+    <col min="19" max="19" width="33.625" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="19.625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16"/>
+    </row>
+    <row r="7" spans="1:19" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="24"/>
+    </row>
+    <row r="9" spans="1:19" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="S9" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="24"/>
+    </row>
+    <row r="11" spans="1:19" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R11" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="S11" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="S12" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R13" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="S13" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" s="24"/>
+    </row>
+    <row r="15" spans="1:19" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R15" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="S15" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13" style="3" customWidth="1"/>
+    <col min="2" max="2" width="76.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9" style="27" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="27" customWidth="1"/>
+    <col min="5" max="5" width="13" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.25" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.75" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>